<commit_message>
Update the case for modification and improvement.
</commit_message>
<xml_diff>
--- a/controller/unity_test/unity_case_example.xlsx
+++ b/controller/unity_test/unity_case_example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>Script Info</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,10 +42,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Function</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Component</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -94,26 +90,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Contact Information</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System Location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Display Temperature</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SetTextValue</t>
   </si>
   <si>
@@ -129,182 +105,134 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Navigate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test_site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Site</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>editButton</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time Service Settings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Navigate to Configuration page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Navigate to System page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Navigate to Time Service page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Access to identity confirmation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum103</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>External Time Source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NTP Time Server</t>
+  </si>
+  <si>
+    <t>enum34</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NTP Time Sync Rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time Zone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable Auto-Sync To Managed Device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Managed Device Auto-Sync Rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chbx31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>submitButton</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Save button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Edit button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.163.230.119</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>System</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Navigate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Celsius</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_site</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test Site</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>editButton</t>
+    <t>System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time Service Settings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Comment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time Service Settings</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Navigate to Configuration page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Navigate to System page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Navigate to Time Service page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time Service Settings</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Access to identity confirmation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enum103</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>External Time Source</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>str33</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NTP Time Server</t>
-  </si>
-  <si>
-    <t>enum34</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NTP Time Sync Rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time Zone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Enable Auto-Sync To Managed Device</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Managed Device Auto-Sync Rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>System Page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enum35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chbx31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enum123</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>submitButton</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_Info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>str4329</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>str4332</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>str4331</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>str4330</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>enum157</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Save button</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Edit button</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10.163.230.119</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BACnet System</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>12 Hours</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(GMT-11:00) UTC-11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -404,7 +332,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -424,6 +352,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -727,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I25" sqref="D16:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -761,16 +692,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -787,7 +718,7 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="16.5">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>26</v>
@@ -795,17 +726,17 @@
       <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>17</v>
+      <c r="D2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -815,19 +746,19 @@
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" ht="16.5">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -839,28 +770,28 @@
     </row>
     <row r="4" spans="1:12" s="4" customFormat="1" ht="16.5">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -869,28 +800,28 @@
     </row>
     <row r="5" spans="1:12" s="4" customFormat="1" ht="16.5">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -899,26 +830,26 @@
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1" ht="16.5">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3">
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -927,24 +858,24 @@
     </row>
     <row r="7" spans="1:12" s="4" customFormat="1" ht="16.5">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="3">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -953,23 +884,23 @@
     </row>
     <row r="8" spans="1:12" s="4" customFormat="1" ht="16.5">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="3">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
+      <c r="D8" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -979,27 +910,29 @@
     </row>
     <row r="9" spans="1:12" s="4" customFormat="1" ht="16.5">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="3">
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="G9" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>70</v>
+        <v>19</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1012,20 +945,20 @@
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -1038,20 +971,20 @@
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>71</v>
+        <v>19</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1064,20 +997,20 @@
         <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>72</v>
+        <v>19</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1090,17 +1023,17 @@
         <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="I13" s="3" t="b">
         <v>1</v>
@@ -1116,20 +1049,20 @@
         <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>71</v>
+        <v>19</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1142,17 +1075,17 @@
         <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
@@ -1165,12 +1098,8 @@
       <c r="C16" s="3">
         <v>15</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1185,21 +1114,11 @@
       <c r="C17" s="3">
         <v>16</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1211,21 +1130,11 @@
       <c r="C18" s="3">
         <v>17</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -1237,19 +1146,11 @@
       <c r="C19" s="3">
         <v>18</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="G19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1259,18 +1160,10 @@
       <c r="C20" s="3">
         <v>19</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -1281,22 +1174,12 @@
       <c r="C21" s="3">
         <v>20</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1305,22 +1188,12 @@
       <c r="C22" s="3">
         <v>21</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1329,22 +1202,12 @@
       <c r="C23" s="3">
         <v>22</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>59</v>
-      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -1353,22 +1216,12 @@
       <c r="C24" s="3">
         <v>23</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -1377,22 +1230,12 @@
       <c r="C25" s="3">
         <v>24</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -1401,19 +1244,11 @@
       <c r="C26" s="3">
         <v>25</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>

</xml_diff>

<commit_message>
Change the test case example(unity_case_example.xlsx) for test.
</commit_message>
<xml_diff>
--- a/controller/unity_test/unity_case_example.xlsx
+++ b/controller/unity_test/unity_case_example.xlsx
@@ -90,9 +90,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SetTextValue</t>
-  </si>
-  <si>
     <t>Select_Combo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -188,10 +185,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>chbx31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>enum123</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -200,10 +193,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Set</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Save button</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -233,6 +222,18 @@
   </si>
   <si>
     <t>Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set_TextValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set_CheckBox</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chkbx31</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -658,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I25" sqref="D16:I25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -692,7 +693,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -727,10 +728,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>16</v>
@@ -746,19 +747,19 @@
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" ht="16.5">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -782,16 +783,16 @@
         <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -812,16 +813,16 @@
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -840,16 +841,16 @@
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -868,14 +869,14 @@
         <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -891,10 +892,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>16</v>
@@ -920,16 +921,16 @@
         <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
@@ -948,17 +949,17 @@
         <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -974,14 +975,14 @@
         <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I11" s="3">
         <v>1</v>
@@ -1000,14 +1001,14 @@
         <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I12" s="3">
         <v>2</v>
@@ -1026,14 +1027,14 @@
         <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="I13" s="3" t="b">
         <v>1</v>
@@ -1052,14 +1053,14 @@
         <v>17</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I14" s="3">
         <v>1</v>
@@ -1078,14 +1079,14 @@
         <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>

</xml_diff>